<commit_message>
Knowledge Rules Implemented Half way
</commit_message>
<xml_diff>
--- a/backend/api/kb/pH-to-NPK.xlsx
+++ b/backend/api/kb/pH-to-NPK.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="9">
-  <si>
-    <t>pH</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="10">
   <si>
     <t>N</t>
   </si>
@@ -42,6 +39,12 @@
   </si>
   <si>
     <t>mid</t>
+  </si>
+  <si>
+    <t>max_pH</t>
+  </si>
+  <si>
+    <t>min_pH</t>
   </si>
 </sst>
 </file>
@@ -870,432 +873,522 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>0.49</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3">
+        <v>0.99</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>1.49</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.5</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="B5">
+        <v>1.99</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6">
+        <v>2.4900000000000002</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.5</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
+      <c r="B7">
+        <v>2.99</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
+      <c r="B8">
+        <v>3.49</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.5</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
+      <c r="B9">
+        <v>3.99</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
+      <c r="B10">
+        <v>4.49</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.5</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
+      <c r="B11">
+        <v>4.99</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
+      <c r="B12">
+        <v>5.49</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5.5</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
+      <c r="B13">
+        <v>5.99</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
+      <c r="B14">
+        <v>6.49</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6.5</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
+      <c r="B15">
+        <v>6.99</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
+      <c r="B16">
+        <v>7.49</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.5</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
+      <c r="B17">
+        <v>7.99</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
+      <c r="B18">
+        <v>8.49</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8.5</v>
       </c>
-      <c r="B19" t="s">
-        <v>8</v>
+      <c r="B19">
+        <v>8.99</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
+      <c r="B20">
+        <v>9.49</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9.5</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
+      <c r="B21">
+        <v>9.99</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
-        <v>4</v>
+      <c r="B22">
+        <v>10.49</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10.5</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
+      <c r="B23">
+        <v>10.99</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
+      <c r="B24">
+        <v>11.49</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11.5</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
+      <c r="B25">
+        <v>11.99</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
-        <v>4</v>
+      <c r="B26">
+        <v>12.49</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12.5</v>
       </c>
-      <c r="B27" t="s">
-        <v>4</v>
+      <c r="B27">
+        <v>12.99</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
+      <c r="B28">
+        <v>13.49</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>13.5</v>
       </c>
-      <c r="B29" t="s">
-        <v>4</v>
+      <c r="B29">
+        <v>13.99</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
+      <c r="B30">
+        <v>14.49</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1315,12 +1408,12 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned Query Success. With "Loading" word in UI.
</commit_message>
<xml_diff>
--- a/backend/api/kb/pH-to-NPK.xlsx
+++ b/backend/api/kb/pH-to-NPK.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="10">
   <si>
     <t>N</t>
   </si>
@@ -873,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -920,7 +920,7 @@
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -954,7 +954,7 @@
         <v>1.5</v>
       </c>
       <c r="B5">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -971,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>2.4900000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -988,7 +988,7 @@
         <v>2.5</v>
       </c>
       <c r="B7">
-        <v>2.99</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -1005,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>3.49</v>
+        <v>3.5</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -1022,7 +1022,7 @@
         <v>3.5</v>
       </c>
       <c r="B9">
-        <v>3.99</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -1039,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>4.49</v>
+        <v>4.5</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1056,7 +1056,7 @@
         <v>4.5</v>
       </c>
       <c r="B11">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -1073,7 +1073,7 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>5.49</v>
+        <v>5.5</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1090,7 +1090,7 @@
         <v>5.5</v>
       </c>
       <c r="B13">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1107,7 +1107,7 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>6.49</v>
+        <v>6.5</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1124,7 +1124,7 @@
         <v>6.5</v>
       </c>
       <c r="B15">
-        <v>6.99</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -1141,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>7.49</v>
+        <v>7.5</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1158,7 +1158,7 @@
         <v>7.5</v>
       </c>
       <c r="B17">
-        <v>7.99</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1175,7 +1175,7 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>8.49</v>
+        <v>8.5</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1192,7 +1192,7 @@
         <v>8.5</v>
       </c>
       <c r="B19">
-        <v>8.99</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1209,7 +1209,7 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>9.49</v>
+        <v>9.5</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1226,7 +1226,7 @@
         <v>9.5</v>
       </c>
       <c r="B21">
-        <v>9.99</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -1243,7 +1243,7 @@
         <v>10</v>
       </c>
       <c r="B22">
-        <v>10.49</v>
+        <v>10.5</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -1260,7 +1260,7 @@
         <v>10.5</v>
       </c>
       <c r="B23">
-        <v>10.99</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -1277,7 +1277,7 @@
         <v>11</v>
       </c>
       <c r="B24">
-        <v>11.49</v>
+        <v>11.5</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -1294,7 +1294,7 @@
         <v>11.5</v>
       </c>
       <c r="B25">
-        <v>11.99</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -1311,7 +1311,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>12.49</v>
+        <v>12.5</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -1328,7 +1328,7 @@
         <v>12.5</v>
       </c>
       <c r="B27">
-        <v>12.99</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -1345,7 +1345,7 @@
         <v>13</v>
       </c>
       <c r="B28">
-        <v>13.49</v>
+        <v>13.5</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -1362,7 +1362,7 @@
         <v>13.5</v>
       </c>
       <c r="B29">
-        <v>13.99</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -1371,23 +1371,6 @@
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>14</v>
-      </c>
-      <c r="B30">
-        <v>14.49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>